<commit_message>
Create updated excel info sheets
</commit_message>
<xml_diff>
--- a/zzz_lib/code and data/data/Excel/lfpbygenderparent.xlsx
+++ b/zzz_lib/code and data/data/Excel/lfpbygenderparent.xlsx
@@ -1,26 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eaf80618f9c5e5a/Work Items/TheCareBoard/zzz_lib/code and data/data/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74B3A8C7-2943-4547-B337-DCDCDDB9D9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{74B3A8C7-2943-4547-B337-DCDCDDB9D9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFC43FD3-092D-4597-B8F1-01B8AEAB8298}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{4905CAB1-AC03-42CF-A0A4-2681C9A0550F}"/>
   </bookViews>
   <sheets>
-    <sheet name="lfpbygenderparent" sheetId="1" r:id="rId1"/>
+    <sheet name="Information" sheetId="3" r:id="rId1"/>
+    <sheet name="lfpbygenderparent" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="18">
   <si>
     <t>year</t>
   </si>
@@ -54,12 +77,54 @@
   <si>
     <t>Other</t>
   </si>
+  <si>
+    <t>Data Scope</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>US Laborforce Participation by Gender and Parenthood, 1990-2024</t>
+  </si>
+  <si>
+    <r>
+      <t> Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Care Board</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, University of Kansas, using microdata from the Current Population Survey (CPS) curated by ipums.org. For more details, visit thecareboard.ku.edu.</t>
+    </r>
+  </si>
+  <si>
+    <t>Monthly observations from 1990 onward for national laborforce participation broken down by genderand parenthood interactions.</t>
+  </si>
+  <si>
+    <t>Definition of labor force participation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We replicate the BLS methodology for labor force participation. LFP includes full-time, part-time, and those actively seeking employment. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +255,66 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,7 +501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -491,8 +616,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -535,11 +697,44 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -577,6 +772,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{6F12A263-FDD0-46D9-B3C4-9B9AB552493E}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -594,6 +790,70 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -912,11 +1172,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61DE90AB-FEB3-44B5-B4F9-08215196400D}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="95.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4F48AC-F3F0-444B-959C-88E567B48A02}">
   <dimension ref="A1:G2086"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D596" sqref="D596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>